<commit_message>
Amplicon seq. pipe results with new amplicon names
</commit_message>
<xml_diff>
--- a/data/20170127_GEP00001/NGSpreliminaryData/SLX-13775.haplotypeCaller.variants.xlsx
+++ b/data/20170127_GEP00001/NGSpreliminaryData/SLX-13775.haplotypeCaller.variants.xlsx
@@ -328,7 +328,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -460,7 +460,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>STAT3.3.off1</t>
+          <t>GRCh37.p13_chr12_125765583</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>STAT3.3.off1</t>
+          <t>GRCh37.p13_chr12_125765583</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>STAT3.1.off1</t>
+          <t>GRCh37.p13_chr1_112991561</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1308,47 +1308,37 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>frameshift</t>
+          <t>intron,non_coding_transcript</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>STAT3</t>
+          <t>TMEM132B</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>c.330_331dupGG</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>p.E111Gfs*28</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>gaa/gGGaa</t>
+          <t>n.32-68308_32-68307delGG</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>chr17</t>
+          <t>chr12</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>4.0497617E7</v>
+        <v>1.25765688E8</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
+          <t>TGG</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>T</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>TCC</t>
-        </is>
-      </c>
       <c r="L2" s="1" t="inlineStr">
         <is>
           <t>IGV</t>
@@ -1365,10 +1355,10 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0.38</v>
+        <v>0.164</v>
       </c>
       <c r="P2" t="n">
-        <v>9596.0</v>
+        <v>9830.0</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -1376,42 +1366,42 @@
         </is>
       </c>
       <c r="R2" t="n">
-        <v>104129.0</v>
+        <v>41763.0</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr12_125765583</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>ENSG00000168610</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>4 of 24</t>
+          <t>ENSG00000139364</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>1 of 1</t>
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>58.0</v>
+        <v>38.0</v>
       </c>
       <c r="AD2" t="n">
-        <v>2.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>ATTCT</t>
+          <t>CCTAG</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>T/TCC</t>
+          <t>TGG/T</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>CCCAC</t>
+          <t>GAAGA</t>
         </is>
       </c>
     </row>
@@ -1428,7 +1418,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>stop_gained,frameshift</t>
+          <t>frameshift</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1438,17 +1428,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>c.329_330insA</t>
+          <t>c.330_331dupGG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>p.W110*</t>
+          <t>p.E111Gfs*28</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>tgg/tgAg</t>
+          <t>gaa/gGGaa</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -1457,16 +1447,16 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>4.0497619E7</v>
+        <v>4.0497617E7</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>T</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>TCC</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr">
@@ -1485,10 +1475,10 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0.616</v>
+        <v>0.38</v>
       </c>
       <c r="P3" t="n">
-        <v>9598.0</v>
+        <v>9596.0</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -1496,11 +1486,11 @@
         </is>
       </c>
       <c r="R3" t="n">
-        <v>176103.0</v>
+        <v>104129.0</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -1514,24 +1504,24 @@
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>60.0</v>
+        <v>58.0</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>TCTTC</t>
+          <t>ATTCT</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>C/CT</t>
+          <t>T/TCC</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>CACAG</t>
+          <t>CCCAC</t>
         </is>
       </c>
     </row>
@@ -1548,35 +1538,45 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>intron,non_coding_transcript</t>
+          <t>stop_gained,frameshift</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TMEM132B</t>
+          <t>STAT3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>n.32-68308_32-68307delGG</t>
+          <t>c.329_330insA</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>p.W110*</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>tgg/tgAg</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>chr12</t>
+          <t>chr17</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1.25765688E8</v>
+        <v>4.0497619E7</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>TGG</t>
+          <t>C</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>CT</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
@@ -1595,10 +1595,10 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0.164</v>
+        <v>0.616</v>
       </c>
       <c r="P4" t="n">
-        <v>9830.0</v>
+        <v>9598.0</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -1606,42 +1606,42 @@
         </is>
       </c>
       <c r="R4" t="n">
-        <v>41763.0</v>
+        <v>176103.0</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>STAT3.3.off1</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>ENSG00000139364</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>1 of 1</t>
+          <t>ENSG00000168610</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>4 of 24</t>
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>38.0</v>
+        <v>60.0</v>
       </c>
       <c r="AD4" t="n">
-        <v>-2.0</v>
+        <v>1.0</v>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>CCTAG</t>
+          <t>TCTTC</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>TGG/T</t>
+          <t>C/CT</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>GAAGA</t>
+          <t>CACAG</t>
         </is>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -2195,7 +2195,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -2795,7 +2795,7 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
@@ -2917,7 +2917,7 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -3397,7 +3397,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -3639,7 +3639,7 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -3999,7 +3999,7 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -4121,7 +4121,7 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -4241,7 +4241,7 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -4601,7 +4601,7 @@
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
@@ -4961,7 +4961,7 @@
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
@@ -5201,7 +5201,7 @@
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
@@ -5441,7 +5441,7 @@
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U36" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U37" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U38" t="inlineStr">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
@@ -5923,7 +5923,7 @@
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U40" t="inlineStr">
@@ -6043,7 +6043,7 @@
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U41" t="inlineStr">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U42" t="inlineStr">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U43" t="inlineStr">
@@ -6403,7 +6403,7 @@
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U44" t="inlineStr">
@@ -6523,7 +6523,7 @@
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U45" t="inlineStr">
@@ -6643,7 +6643,7 @@
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U46" t="inlineStr">
@@ -6763,7 +6763,7 @@
       </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U47" t="inlineStr">
@@ -6883,7 +6883,7 @@
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U48" t="inlineStr">
@@ -7003,7 +7003,7 @@
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U49" t="inlineStr">
@@ -7123,7 +7123,7 @@
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U50" t="inlineStr">
@@ -7243,7 +7243,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U51" t="inlineStr">
@@ -7363,7 +7363,7 @@
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U52" t="inlineStr">
@@ -7483,7 +7483,7 @@
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U53" t="inlineStr">
@@ -7603,7 +7603,7 @@
       </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U54" t="inlineStr">
@@ -7723,7 +7723,7 @@
       </c>
       <c r="S55" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U55" t="inlineStr">
@@ -7843,7 +7843,7 @@
       </c>
       <c r="S56" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U56" t="inlineStr">
@@ -7963,7 +7963,7 @@
       </c>
       <c r="S57" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U57" t="inlineStr">
@@ -8083,7 +8083,7 @@
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U58" t="inlineStr">
@@ -8203,7 +8203,7 @@
       </c>
       <c r="S59" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U59" t="inlineStr">
@@ -8325,7 +8325,7 @@
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U60" t="inlineStr">
@@ -8445,7 +8445,7 @@
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U61" t="inlineStr">
@@ -8565,7 +8565,7 @@
       </c>
       <c r="S62" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U62" t="inlineStr">
@@ -8685,7 +8685,7 @@
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U63" t="inlineStr">
@@ -8805,7 +8805,7 @@
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U64" t="inlineStr">
@@ -8925,7 +8925,7 @@
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U65" t="inlineStr">
@@ -9045,7 +9045,7 @@
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U66" t="inlineStr">
@@ -9165,7 +9165,7 @@
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U67" t="inlineStr">
@@ -9285,7 +9285,7 @@
       </c>
       <c r="S68" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
@@ -9405,7 +9405,7 @@
       </c>
       <c r="S69" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U69" t="inlineStr">
@@ -9525,7 +9525,7 @@
       </c>
       <c r="S70" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U70" t="inlineStr">
@@ -9645,7 +9645,7 @@
       </c>
       <c r="S71" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U71" t="inlineStr">
@@ -9765,7 +9765,7 @@
       </c>
       <c r="S72" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U72" t="inlineStr">
@@ -9885,7 +9885,7 @@
       </c>
       <c r="S73" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U73" t="inlineStr">
@@ -10005,7 +10005,7 @@
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U74" t="inlineStr">
@@ -10125,7 +10125,7 @@
       </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U75" t="inlineStr">
@@ -10245,7 +10245,7 @@
       </c>
       <c r="S76" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U76" t="inlineStr">
@@ -10365,7 +10365,7 @@
       </c>
       <c r="S77" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U77" t="inlineStr">
@@ -10485,7 +10485,7 @@
       </c>
       <c r="S78" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U78" t="inlineStr">
@@ -10605,7 +10605,7 @@
       </c>
       <c r="S79" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U79" t="inlineStr">
@@ -10725,7 +10725,7 @@
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U80" t="inlineStr">
@@ -10845,7 +10845,7 @@
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U81" t="inlineStr">
@@ -10965,7 +10965,7 @@
       </c>
       <c r="S82" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U82" t="inlineStr">
@@ -11085,7 +11085,7 @@
       </c>
       <c r="S83" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U83" t="inlineStr">
@@ -11205,7 +11205,7 @@
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U84" t="inlineStr">
@@ -11325,7 +11325,7 @@
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U85" t="inlineStr">
@@ -11445,7 +11445,7 @@
       </c>
       <c r="S86" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U86" t="inlineStr">
@@ -11565,7 +11565,7 @@
       </c>
       <c r="S87" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U87" t="inlineStr">
@@ -11685,7 +11685,7 @@
       </c>
       <c r="S88" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U88" t="inlineStr">
@@ -11805,7 +11805,7 @@
       </c>
       <c r="S89" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U89" t="inlineStr">
@@ -11925,7 +11925,7 @@
       </c>
       <c r="S90" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U90" t="inlineStr">
@@ -12045,7 +12045,7 @@
       </c>
       <c r="S91" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U91" t="inlineStr">
@@ -12165,7 +12165,7 @@
       </c>
       <c r="S92" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U92" t="inlineStr">
@@ -12223,17 +12223,17 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>c.164_167delTGGT</t>
+          <t>c.314_315delTG</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>p.L55Cfs*82</t>
+          <t>p.V105Gfs*66</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>tTGGTg/tg</t>
+          <t>gTG/g</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -12242,16 +12242,16 @@
         </is>
       </c>
       <c r="I93" t="n">
-        <v>4.0498692E7</v>
+        <v>4.0497633E7</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>CACCA</t>
+          <t>CCA</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>C,CTCA</t>
         </is>
       </c>
       <c r="L93" s="1" t="inlineStr">
@@ -12270,10 +12270,10 @@
         </is>
       </c>
       <c r="O93" t="n">
-        <v>0.996</v>
+        <v>0.405</v>
       </c>
       <c r="P93" t="n">
-        <v>9713.0</v>
+        <v>343.0</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
@@ -12281,11 +12281,11 @@
         </is>
       </c>
       <c r="R93" t="n">
-        <v>387841.0</v>
+        <v>10293.0</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U93" t="inlineStr">
@@ -12295,28 +12295,30 @@
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>3 of 24</t>
+          <t>4 of 24</t>
         </is>
       </c>
       <c r="AC93" t="n">
-        <v>54.0</v>
-      </c>
-      <c r="AD93" t="n">
-        <v>-4.0</v>
+        <v>74.0</v>
+      </c>
+      <c r="AD93" t="inlineStr">
+        <is>
+          <t>-2,1</t>
+        </is>
       </c>
       <c r="AE93" t="inlineStr">
         <is>
-          <t>TGAAA</t>
+          <t>CCGGG</t>
         </is>
       </c>
       <c r="AF93" t="inlineStr">
         <is>
-          <t>CACCA/C</t>
+          <t>CCA/C,CTCA</t>
         </is>
       </c>
       <c r="AG93" t="inlineStr">
         <is>
-          <t>AAGTG</t>
+          <t>CAATC</t>
         </is>
       </c>
     </row>
@@ -12343,17 +12345,17 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>c.314_315delTG</t>
+          <t>c.164_167delTGGT</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>p.V105Gfs*66</t>
+          <t>p.L55Cfs*82</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>gTG/g</t>
+          <t>tTGGTg/tg</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -12362,16 +12364,16 @@
         </is>
       </c>
       <c r="I94" t="n">
-        <v>4.0497633E7</v>
+        <v>4.0498692E7</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>CCA</t>
+          <t>CACCA</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>C,CTCA</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L94" s="1" t="inlineStr">
@@ -12390,10 +12392,10 @@
         </is>
       </c>
       <c r="O94" t="n">
-        <v>0.405</v>
+        <v>0.996</v>
       </c>
       <c r="P94" t="n">
-        <v>343.0</v>
+        <v>9713.0</v>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
@@ -12401,11 +12403,11 @@
         </is>
       </c>
       <c r="R94" t="n">
-        <v>10293.0</v>
+        <v>387841.0</v>
       </c>
       <c r="S94" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U94" t="inlineStr">
@@ -12415,30 +12417,28 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>4 of 24</t>
+          <t>3 of 24</t>
         </is>
       </c>
       <c r="AC94" t="n">
-        <v>74.0</v>
-      </c>
-      <c r="AD94" t="inlineStr">
-        <is>
-          <t>-2,1</t>
-        </is>
+        <v>54.0</v>
+      </c>
+      <c r="AD94" t="n">
+        <v>-4.0</v>
       </c>
       <c r="AE94" t="inlineStr">
         <is>
-          <t>CCGGG</t>
+          <t>TGAAA</t>
         </is>
       </c>
       <c r="AF94" t="inlineStr">
         <is>
-          <t>CCA/C,CTCA</t>
+          <t>CACCA/C</t>
         </is>
       </c>
       <c r="AG94" t="inlineStr">
         <is>
-          <t>CAATC</t>
+          <t>AAGTG</t>
         </is>
       </c>
     </row>
@@ -12527,7 +12527,7 @@
       </c>
       <c r="S95" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U95" t="inlineStr">
@@ -12647,7 +12647,7 @@
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>STAT3.1.in</t>
+          <t>GRCh37.p13_chr17_40498615</t>
         </is>
       </c>
       <c r="U96" t="inlineStr">
@@ -12767,7 +12767,7 @@
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U97" t="inlineStr">
@@ -12887,7 +12887,7 @@
       </c>
       <c r="S98" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U98" t="inlineStr">
@@ -13007,7 +13007,7 @@
       </c>
       <c r="S99" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U99" t="inlineStr">
@@ -13127,7 +13127,7 @@
       </c>
       <c r="S100" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U100" t="inlineStr">
@@ -13249,7 +13249,7 @@
       </c>
       <c r="S101" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U101" t="inlineStr">
@@ -13369,7 +13369,7 @@
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U102" t="inlineStr">
@@ -13489,7 +13489,7 @@
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U103" t="inlineStr">
@@ -13609,7 +13609,7 @@
       </c>
       <c r="S104" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U104" t="inlineStr">
@@ -13729,7 +13729,7 @@
       </c>
       <c r="S105" t="inlineStr">
         <is>
-          <t>STAT3.2.in__STAT3.3.in__STAT3.4.in</t>
+          <t>GRCh37.p13_chr17_40497540</t>
         </is>
       </c>
       <c r="U105" t="inlineStr">

</xml_diff>